<commit_message>
Update LED2 value as DNP + Manually Update BOM
</commit_message>
<xml_diff>
--- a/apollo-board_TPS63060/manufacturing/BOM/BOM.xlsx
+++ b/apollo-board_TPS63060/manufacturing/BOM/BOM.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="516" yWindow="576" windowWidth="21852" windowHeight="9204"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Tabellenblatt1" sheetId="1" r:id="rId4"/>
+    <sheet name="Tabellenblatt1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="136">
   <si>
     <t>References</t>
   </si>
@@ -316,9 +319,6 @@
     <t>LED2</t>
   </si>
   <si>
-    <t>150060YS75000_0603</t>
-  </si>
-  <si>
     <t>JP2</t>
   </si>
   <si>
@@ -419,26 +419,33 @@
   </si>
   <si>
     <t>PinSocket_1x13_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>DNP/150060YS75000_0603</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -448,7 +455,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -458,38 +465,40 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -679,25 +688,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="5.0"/>
-    <col customWidth="1" min="3" max="3" width="29.86"/>
-    <col customWidth="1" min="4" max="4" width="55.71"/>
+    <col min="1" max="1" width="43.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="3" width="29.88671875" customWidth="1"/>
+    <col min="4" max="4" width="55.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -714,12 +729,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -728,12 +743,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>9</v>
@@ -742,12 +757,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
@@ -756,12 +771,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>13</v>
@@ -770,12 +785,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
@@ -784,12 +799,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>17</v>
@@ -798,12 +813,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>19</v>
@@ -812,12 +827,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>21</v>
@@ -826,12 +841,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>24</v>
@@ -840,12 +855,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>26</v>
@@ -854,12 +869,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>28</v>
@@ -868,12 +883,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>31</v>
@@ -882,12 +897,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>34</v>
@@ -896,12 +911,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B15" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>36</v>
@@ -913,12 +928,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B16" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>38</v>
@@ -927,12 +942,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B17" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>40</v>
@@ -941,12 +956,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B18" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>42</v>
@@ -955,12 +970,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B19" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>44</v>
@@ -969,12 +984,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B20" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>46</v>
@@ -983,12 +998,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B21" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>48</v>
@@ -997,12 +1012,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B22" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>50</v>
@@ -1011,12 +1026,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B23" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>52</v>
@@ -1028,12 +1043,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B24" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>54</v>
@@ -1042,12 +1057,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B25" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>56</v>
@@ -1056,12 +1071,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B26" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>58</v>
@@ -1070,12 +1085,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B27" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>60</v>
@@ -1084,12 +1099,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B28" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>63</v>
@@ -1098,12 +1113,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B29" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>65</v>
@@ -1112,12 +1127,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B30" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>67</v>
@@ -1126,12 +1141,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B31" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>70</v>
@@ -1140,12 +1155,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B32" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>72</v>
@@ -1154,12 +1169,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B33" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>75</v>
@@ -1168,12 +1183,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B34" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>78</v>
@@ -1182,12 +1197,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B35" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>81</v>
@@ -1196,12 +1211,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B36" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>84</v>
@@ -1210,12 +1225,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B37" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>87</v>
@@ -1224,12 +1239,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B38" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>90</v>
@@ -1238,12 +1253,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B39" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>93</v>
@@ -1252,12 +1267,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B40" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>96</v>
@@ -1266,12 +1281,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>97</v>
       </c>
       <c r="B41" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>98</v>
@@ -1280,218 +1295,221 @@
         <v>99</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B42" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>101</v>
+        <v>135</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="43">
+      <c r="E42" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B43" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B44" s="2">
+        <v>4</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B44" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D44" s="2" t="s">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="2" t="s">
+      <c r="B45" s="2">
+        <v>2</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B45" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="2" t="s">
+      <c r="B46" s="2">
+        <v>1</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B46" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C46" s="2" t="s">
+      <c r="D46" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="2" t="s">
+      <c r="B47" s="2">
+        <v>4</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="B47" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48" s="2">
+        <v>1</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="B48" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>115</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B49" s="2">
+        <v>1</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B49" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C49" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D49" s="2" t="s">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="2" t="s">
+      <c r="B50" s="2">
+        <v>1</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B50" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C50" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D50" s="2" t="s">
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="2" t="s">
+      <c r="B51" s="2">
+        <v>1</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B51" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C51" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B52" s="2">
+        <v>1</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B52" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C52" s="2" t="s">
+      <c r="D52" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B53" s="2">
+        <v>1</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B53" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="D53" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B54" s="2">
+        <v>1</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B54" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C54" s="2" t="s">
+      <c r="D54" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B55" s="2">
+        <v>1</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B55" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C55" s="2" t="s">
+      <c r="D55" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>135</v>
-      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>